<commit_message>
cambios en JAVAde Sistemas Operativo
Corregí el algoritmo fifo orientado a objeto
Y la Guía de estudio Nro 1 completo por Pablo Miranda
</commit_message>
<xml_diff>
--- a/Introducción a los Sistemas Operativos/Guías de Estudio/IaSO-Guia-de-Trabajos-Practicos.xlsx
+++ b/Introducción a los Sistemas Operativos/Guías de Estudio/IaSO-Guia-de-Trabajos-Practicos.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="33">
   <si>
     <t xml:space="preserve">a) Prioridades (No Apropitativo). </t>
   </si>
@@ -119,9 +119,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Revisar. No sé si está bien¿?</t>
-  </si>
-  <si>
     <t xml:space="preserve">c) Shortest Remaining Time (Apropitativo). </t>
   </si>
 </sst>
@@ -173,7 +170,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,12 +192,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -250,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -287,25 +278,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -314,15 +314,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="R39" sqref="R39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,7 +704,7 @@
       <c r="AD3" s="7">
         <v>29</v>
       </c>
-      <c r="AE3" s="36">
+      <c r="AE3" s="28">
         <v>30</v>
       </c>
       <c r="AF3" s="7">
@@ -796,7 +790,7 @@
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
       <c r="AD4" s="6"/>
-      <c r="AE4" s="37"/>
+      <c r="AE4" s="29"/>
       <c r="AF4" s="6"/>
       <c r="AG4" s="6"/>
       <c r="AH4" s="6"/>
@@ -858,7 +852,7 @@
       <c r="AD5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="AE5" s="36" t="s">
+      <c r="AE5" s="28" t="s">
         <v>10</v>
       </c>
       <c r="AF5" s="6"/>
@@ -922,7 +916,7 @@
       <c r="AB6" s="6"/>
       <c r="AC6" s="6"/>
       <c r="AD6" s="6"/>
-      <c r="AE6" s="37"/>
+      <c r="AE6" s="29"/>
       <c r="AF6" s="6"/>
       <c r="AG6" s="6"/>
       <c r="AH6" s="6"/>
@@ -988,7 +982,7 @@
       </c>
       <c r="AC7" s="6"/>
       <c r="AD7" s="6"/>
-      <c r="AE7" s="37"/>
+      <c r="AE7" s="29"/>
       <c r="AF7" s="6"/>
       <c r="AG7" s="6"/>
       <c r="AH7" s="6"/>
@@ -1050,7 +1044,7 @@
       <c r="AB8" s="6"/>
       <c r="AC8" s="6"/>
       <c r="AD8" s="6"/>
-      <c r="AE8" s="37"/>
+      <c r="AE8" s="29"/>
       <c r="AF8" s="6"/>
       <c r="AG8" s="6"/>
       <c r="AH8" s="6"/>
@@ -1088,30 +1082,30 @@
       <c r="C11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P11" s="24" t="s">
+      <c r="P11" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24" t="s">
+      <c r="Q11" s="34"/>
+      <c r="R11" s="34"/>
+      <c r="S11" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="T11" s="24"/>
-      <c r="U11" s="24"/>
-      <c r="V11" s="26" t="s">
+      <c r="T11" s="34"/>
+      <c r="U11" s="34"/>
+      <c r="V11" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="W11" s="26"/>
-      <c r="X11" s="26"/>
-      <c r="Y11" s="26"/>
-      <c r="Z11" s="21" t="s">
+      <c r="W11" s="32"/>
+      <c r="X11" s="32"/>
+      <c r="Y11" s="32"/>
+      <c r="Z11" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="AA11" s="21"/>
-      <c r="AB11" s="21"/>
-      <c r="AC11" s="21"/>
-      <c r="AD11" s="21"/>
-      <c r="AE11" s="21"/>
+      <c r="AA11" s="33"/>
+      <c r="AB11" s="33"/>
+      <c r="AC11" s="33"/>
+      <c r="AD11" s="33"/>
+      <c r="AE11" s="33"/>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
@@ -1120,28 +1114,28 @@
       <c r="B12" t="s">
         <v>3</v>
       </c>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="24"/>
-      <c r="S12" s="24"/>
-      <c r="T12" s="24"/>
-      <c r="U12" s="24"/>
-      <c r="V12" s="26"/>
-      <c r="W12" s="26"/>
-      <c r="X12" s="26"/>
-      <c r="Y12" s="26"/>
-      <c r="Z12" s="21" t="s">
+      <c r="P12" s="34"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="34"/>
+      <c r="S12" s="34"/>
+      <c r="T12" s="34"/>
+      <c r="U12" s="34"/>
+      <c r="V12" s="32"/>
+      <c r="W12" s="32"/>
+      <c r="X12" s="32"/>
+      <c r="Y12" s="32"/>
+      <c r="Z12" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="AA12" s="21"/>
-      <c r="AB12" s="21" t="s">
+      <c r="AA12" s="33"/>
+      <c r="AB12" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="AC12" s="21"/>
-      <c r="AD12" s="21" t="s">
+      <c r="AC12" s="33"/>
+      <c r="AD12" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="AE12" s="21"/>
+      <c r="AE12" s="33"/>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
@@ -1156,34 +1150,34 @@
       <c r="D13" t="s">
         <v>3</v>
       </c>
-      <c r="P13" s="21" t="s">
+      <c r="P13" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="21"/>
-      <c r="S13" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="T13" s="21"/>
-      <c r="U13" s="21"/>
-      <c r="V13" s="21" t="s">
+      <c r="Q13" s="33"/>
+      <c r="R13" s="33"/>
+      <c r="S13" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="T13" s="33"/>
+      <c r="U13" s="33"/>
+      <c r="V13" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="W13" s="21"/>
-      <c r="X13" s="21"/>
-      <c r="Y13" s="21"/>
-      <c r="Z13" s="21">
+      <c r="W13" s="33"/>
+      <c r="X13" s="33"/>
+      <c r="Y13" s="33"/>
+      <c r="Z13" s="33">
         <v>4</v>
       </c>
-      <c r="AA13" s="21"/>
-      <c r="AB13" s="21">
-        <v>3</v>
-      </c>
-      <c r="AC13" s="21"/>
-      <c r="AD13" s="21">
-        <v>3</v>
-      </c>
-      <c r="AE13" s="21"/>
+      <c r="AA13" s="33"/>
+      <c r="AB13" s="33">
+        <v>3</v>
+      </c>
+      <c r="AC13" s="33"/>
+      <c r="AD13" s="33">
+        <v>3</v>
+      </c>
+      <c r="AE13" s="33"/>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
@@ -1198,34 +1192,34 @@
       <c r="D14" t="s">
         <v>3</v>
       </c>
-      <c r="P14" s="21" t="s">
+      <c r="P14" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="21"/>
-      <c r="S14" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="T14" s="21"/>
-      <c r="U14" s="21"/>
-      <c r="V14" s="21" t="s">
+      <c r="Q14" s="33"/>
+      <c r="R14" s="33"/>
+      <c r="S14" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="T14" s="33"/>
+      <c r="U14" s="33"/>
+      <c r="V14" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="W14" s="21"/>
-      <c r="X14" s="21"/>
-      <c r="Y14" s="21"/>
-      <c r="Z14" s="21">
-        <v>2</v>
-      </c>
-      <c r="AA14" s="21"/>
-      <c r="AB14" s="21">
+      <c r="W14" s="33"/>
+      <c r="X14" s="33"/>
+      <c r="Y14" s="33"/>
+      <c r="Z14" s="33">
+        <v>2</v>
+      </c>
+      <c r="AA14" s="33"/>
+      <c r="AB14" s="33">
         <v>4</v>
       </c>
-      <c r="AC14" s="21"/>
-      <c r="AD14" s="21">
-        <v>3</v>
-      </c>
-      <c r="AE14" s="21"/>
+      <c r="AC14" s="33"/>
+      <c r="AD14" s="33">
+        <v>3</v>
+      </c>
+      <c r="AE14" s="33"/>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
@@ -1243,34 +1237,34 @@
       <c r="E15" t="s">
         <v>3</v>
       </c>
-      <c r="P15" s="21" t="s">
+      <c r="P15" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="Q15" s="21"/>
-      <c r="R15" s="21"/>
-      <c r="S15" s="21" t="s">
+      <c r="Q15" s="33"/>
+      <c r="R15" s="33"/>
+      <c r="S15" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="T15" s="21"/>
-      <c r="U15" s="21"/>
-      <c r="V15" s="21" t="s">
+      <c r="T15" s="33"/>
+      <c r="U15" s="33"/>
+      <c r="V15" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="W15" s="21"/>
-      <c r="X15" s="21"/>
-      <c r="Y15" s="21"/>
-      <c r="Z15" s="21">
-        <v>2</v>
-      </c>
-      <c r="AA15" s="21"/>
-      <c r="AB15" s="21">
-        <v>5</v>
-      </c>
-      <c r="AC15" s="21"/>
-      <c r="AD15" s="21">
+      <c r="W15" s="33"/>
+      <c r="X15" s="33"/>
+      <c r="Y15" s="33"/>
+      <c r="Z15" s="33">
+        <v>2</v>
+      </c>
+      <c r="AA15" s="33"/>
+      <c r="AB15" s="33">
+        <v>5</v>
+      </c>
+      <c r="AC15" s="33"/>
+      <c r="AD15" s="33">
         <v>1</v>
       </c>
-      <c r="AE15" s="21"/>
+      <c r="AE15" s="33"/>
     </row>
     <row r="16" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
@@ -1285,34 +1279,34 @@
       <c r="D16" t="s">
         <v>3</v>
       </c>
-      <c r="P16" s="21" t="s">
+      <c r="P16" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="21"/>
-      <c r="S16" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="T16" s="21"/>
-      <c r="U16" s="21"/>
-      <c r="V16" s="21" t="s">
+      <c r="Q16" s="33"/>
+      <c r="R16" s="33"/>
+      <c r="S16" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="T16" s="33"/>
+      <c r="U16" s="33"/>
+      <c r="V16" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="W16" s="21"/>
-      <c r="X16" s="21"/>
-      <c r="Y16" s="21"/>
-      <c r="Z16" s="21">
+      <c r="W16" s="33"/>
+      <c r="X16" s="33"/>
+      <c r="Y16" s="33"/>
+      <c r="Z16" s="33">
         <v>1</v>
       </c>
-      <c r="AA16" s="21"/>
-      <c r="AB16" s="21">
+      <c r="AA16" s="33"/>
+      <c r="AB16" s="33">
         <v>4</v>
       </c>
-      <c r="AC16" s="21"/>
-      <c r="AD16" s="21">
-        <v>5</v>
-      </c>
-      <c r="AE16" s="21"/>
+      <c r="AC16" s="33"/>
+      <c r="AD16" s="33">
+        <v>5</v>
+      </c>
+      <c r="AE16" s="33"/>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
@@ -1327,34 +1321,34 @@
       <c r="D17" t="s">
         <v>3</v>
       </c>
-      <c r="P17" s="21" t="s">
+      <c r="P17" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="Q17" s="21"/>
-      <c r="R17" s="21"/>
-      <c r="S17" s="21" t="s">
+      <c r="Q17" s="33"/>
+      <c r="R17" s="33"/>
+      <c r="S17" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="T17" s="21"/>
-      <c r="U17" s="21"/>
-      <c r="V17" s="21" t="s">
+      <c r="T17" s="33"/>
+      <c r="U17" s="33"/>
+      <c r="V17" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="W17" s="21"/>
-      <c r="X17" s="21"/>
-      <c r="Y17" s="21"/>
-      <c r="Z17" s="21">
-        <v>3</v>
-      </c>
-      <c r="AA17" s="21"/>
-      <c r="AB17" s="21">
-        <v>2</v>
-      </c>
-      <c r="AC17" s="21"/>
-      <c r="AD17" s="21">
-        <v>3</v>
-      </c>
-      <c r="AE17" s="21"/>
+      <c r="W17" s="33"/>
+      <c r="X17" s="33"/>
+      <c r="Y17" s="33"/>
+      <c r="Z17" s="33">
+        <v>3</v>
+      </c>
+      <c r="AA17" s="33"/>
+      <c r="AB17" s="33">
+        <v>2</v>
+      </c>
+      <c r="AC17" s="33"/>
+      <c r="AD17" s="33">
+        <v>3</v>
+      </c>
+      <c r="AE17" s="33"/>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
@@ -1604,7 +1598,7 @@
       <c r="A41" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B41" s="34">
+      <c r="B41" s="26">
         <f>A40</f>
         <v>30</v>
       </c>
@@ -1612,67 +1606,65 @@
     <row r="42" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
     </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>13</v>
       </c>
       <c r="J43" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="N43" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="O43" s="22"/>
-      <c r="P43" s="22"/>
-      <c r="Q43" s="22"/>
-      <c r="R43" s="22"/>
-      <c r="S43" s="22"/>
-      <c r="T43" s="22"/>
-      <c r="U43" s="22"/>
-      <c r="V43" s="22"/>
-      <c r="W43" s="22"/>
-      <c r="X43" s="22"/>
-      <c r="Y43" s="22"/>
-      <c r="Z43" s="22"/>
-      <c r="AA43" s="22"/>
-      <c r="AB43" s="22"/>
-      <c r="AC43" s="22"/>
-      <c r="AD43" s="22"/>
-      <c r="AE43" s="22"/>
-      <c r="AF43" s="22"/>
-      <c r="AG43" s="22"/>
-      <c r="AH43" s="22"/>
-      <c r="AI43" s="22"/>
-      <c r="AJ43" s="22"/>
-      <c r="AK43" s="22"/>
-      <c r="AL43" s="22"/>
-    </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="N44" s="22"/>
-      <c r="O44" s="22"/>
-      <c r="P44" s="22"/>
-      <c r="Q44" s="22"/>
-      <c r="R44" s="22"/>
-      <c r="S44" s="22"/>
-      <c r="T44" s="22"/>
-      <c r="U44" s="22"/>
-      <c r="V44" s="22"/>
-      <c r="W44" s="22"/>
-      <c r="X44" s="22"/>
-      <c r="Y44" s="22"/>
-      <c r="Z44" s="22"/>
-      <c r="AA44" s="22"/>
-      <c r="AB44" s="22"/>
-      <c r="AC44" s="22"/>
-      <c r="AD44" s="22"/>
-      <c r="AE44" s="22"/>
-      <c r="AF44" s="22"/>
-      <c r="AG44" s="22"/>
-      <c r="AH44" s="22"/>
-      <c r="AI44" s="22"/>
-      <c r="AJ44" s="22"/>
-      <c r="AK44" s="22"/>
-      <c r="AL44" s="22"/>
+      <c r="N43" s="38"/>
+      <c r="O43" s="38"/>
+      <c r="P43" s="38"/>
+      <c r="Q43" s="38"/>
+      <c r="R43" s="38"/>
+      <c r="S43" s="38"/>
+      <c r="T43" s="38"/>
+      <c r="U43" s="38"/>
+      <c r="V43" s="38"/>
+      <c r="W43" s="38"/>
+      <c r="X43" s="38"/>
+      <c r="Y43" s="38"/>
+      <c r="Z43" s="38"/>
+      <c r="AA43" s="38"/>
+      <c r="AB43" s="38"/>
+      <c r="AC43" s="38"/>
+      <c r="AD43" s="38"/>
+      <c r="AE43" s="38"/>
+      <c r="AF43" s="38"/>
+      <c r="AG43" s="38"/>
+      <c r="AH43" s="38"/>
+      <c r="AI43" s="38"/>
+      <c r="AJ43" s="38"/>
+      <c r="AK43" s="38"/>
+      <c r="AL43" s="38"/>
+    </row>
+    <row r="44" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N44" s="38"/>
+      <c r="O44" s="38"/>
+      <c r="P44" s="38"/>
+      <c r="Q44" s="38"/>
+      <c r="R44" s="38"/>
+      <c r="S44" s="38"/>
+      <c r="T44" s="38"/>
+      <c r="U44" s="38"/>
+      <c r="V44" s="38"/>
+      <c r="W44" s="38"/>
+      <c r="X44" s="38"/>
+      <c r="Y44" s="38"/>
+      <c r="Z44" s="38"/>
+      <c r="AA44" s="38"/>
+      <c r="AB44" s="38"/>
+      <c r="AC44" s="38"/>
+      <c r="AD44" s="38"/>
+      <c r="AE44" s="38"/>
+      <c r="AF44" s="38"/>
+      <c r="AG44" s="38"/>
+      <c r="AH44" s="38"/>
+      <c r="AI44" s="38"/>
+      <c r="AJ44" s="38"/>
+      <c r="AK44" s="38"/>
+      <c r="AL44" s="38"/>
     </row>
     <row r="45" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
@@ -1714,79 +1706,79 @@
       <c r="M45" s="7">
         <v>12</v>
       </c>
-      <c r="N45" s="7">
+      <c r="N45" s="21">
         <v>13</v>
       </c>
-      <c r="O45" s="7">
+      <c r="O45" s="21">
         <v>14</v>
       </c>
-      <c r="P45" s="7">
+      <c r="P45" s="21">
         <v>15</v>
       </c>
-      <c r="Q45" s="7">
+      <c r="Q45" s="21">
         <v>16</v>
       </c>
-      <c r="R45" s="7">
+      <c r="R45" s="21">
         <v>17</v>
       </c>
-      <c r="S45" s="7">
+      <c r="S45" s="21">
         <v>18</v>
       </c>
-      <c r="T45" s="7">
+      <c r="T45" s="21">
         <v>19</v>
       </c>
-      <c r="U45" s="7">
+      <c r="U45" s="21">
         <v>20</v>
       </c>
-      <c r="V45" s="7">
+      <c r="V45" s="21">
         <v>21</v>
       </c>
-      <c r="W45" s="7">
+      <c r="W45" s="21">
         <v>22</v>
       </c>
-      <c r="X45" s="7">
+      <c r="X45" s="21">
         <v>23</v>
       </c>
-      <c r="Y45" s="7">
+      <c r="Y45" s="21">
         <v>24</v>
       </c>
-      <c r="Z45" s="7">
+      <c r="Z45" s="21">
         <v>25</v>
       </c>
-      <c r="AA45" s="7">
+      <c r="AA45" s="21">
         <v>26</v>
       </c>
-      <c r="AB45" s="7">
+      <c r="AB45" s="21">
         <v>27</v>
       </c>
-      <c r="AC45" s="36">
+      <c r="AC45" s="28">
         <v>28</v>
       </c>
-      <c r="AD45" s="7">
+      <c r="AD45" s="21">
         <v>29</v>
       </c>
-      <c r="AE45" s="7">
+      <c r="AE45" s="21">
         <v>30</v>
       </c>
-      <c r="AF45" s="7">
+      <c r="AF45" s="21">
         <v>31</v>
       </c>
-      <c r="AG45" s="7">
+      <c r="AG45" s="21">
         <v>32</v>
       </c>
-      <c r="AH45" s="7">
+      <c r="AH45" s="21">
         <v>33</v>
       </c>
-      <c r="AI45" s="7">
+      <c r="AI45" s="21">
         <v>34</v>
       </c>
-      <c r="AJ45" s="7">
+      <c r="AJ45" s="21">
         <v>35</v>
       </c>
-      <c r="AK45" s="7">
+      <c r="AK45" s="21">
         <v>36</v>
       </c>
-      <c r="AL45" s="7">
+      <c r="AL45" s="21">
         <v>37</v>
       </c>
       <c r="AM45" s="7">
@@ -1842,7 +1834,7 @@
       <c r="AB46" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="AC46" s="36" t="s">
+      <c r="AC46" s="28" t="s">
         <v>10</v>
       </c>
       <c r="AD46" s="7"/>
@@ -1908,7 +1900,7 @@
       <c r="Z47" s="7"/>
       <c r="AA47" s="7"/>
       <c r="AB47" s="7"/>
-      <c r="AC47" s="36"/>
+      <c r="AC47" s="28"/>
       <c r="AD47" s="7"/>
       <c r="AE47" s="7"/>
       <c r="AF47" s="7"/>
@@ -1970,7 +1962,7 @@
       <c r="Z48" s="7"/>
       <c r="AA48" s="7"/>
       <c r="AB48" s="7"/>
-      <c r="AC48" s="36"/>
+      <c r="AC48" s="28"/>
       <c r="AD48" s="7"/>
       <c r="AE48" s="7"/>
       <c r="AF48" s="7"/>
@@ -2036,7 +2028,7 @@
       <c r="Z49" s="7"/>
       <c r="AA49" s="7"/>
       <c r="AB49" s="7"/>
-      <c r="AC49" s="36"/>
+      <c r="AC49" s="28"/>
       <c r="AD49" s="7"/>
       <c r="AE49" s="7"/>
       <c r="AF49" s="7"/>
@@ -2098,7 +2090,7 @@
       </c>
       <c r="AA50" s="7"/>
       <c r="AB50" s="7"/>
-      <c r="AC50" s="36"/>
+      <c r="AC50" s="28"/>
       <c r="AD50" s="7"/>
       <c r="AE50" s="7"/>
       <c r="AF50" s="7"/>
@@ -2115,11 +2107,11 @@
       <c r="A52" t="s">
         <v>12</v>
       </c>
-      <c r="P52" s="27" t="s">
+      <c r="P52" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="Q52" s="27"/>
-      <c r="R52" s="27"/>
+      <c r="Q52" s="35"/>
+      <c r="R52" s="35"/>
     </row>
     <row r="53" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
@@ -2131,35 +2123,35 @@
       <c r="C53" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P53" s="25" t="s">
+      <c r="P53" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="Q53" s="25"/>
-      <c r="R53" s="25"/>
-      <c r="S53" s="24" t="s">
+      <c r="Q53" s="30"/>
+      <c r="R53" s="30"/>
+      <c r="S53" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="T53" s="24"/>
-      <c r="U53" s="24"/>
-      <c r="V53" s="26" t="s">
+      <c r="T53" s="34"/>
+      <c r="U53" s="34"/>
+      <c r="V53" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="W53" s="26"/>
-      <c r="X53" s="26"/>
-      <c r="Y53" s="26"/>
-      <c r="Z53" s="21" t="s">
+      <c r="W53" s="32"/>
+      <c r="X53" s="32"/>
+      <c r="Y53" s="32"/>
+      <c r="Z53" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="AA53" s="21"/>
-      <c r="AB53" s="21"/>
-      <c r="AC53" s="21"/>
-      <c r="AD53" s="21"/>
-      <c r="AE53" s="21"/>
-      <c r="AF53" s="24" t="s">
+      <c r="AA53" s="33"/>
+      <c r="AB53" s="33"/>
+      <c r="AC53" s="33"/>
+      <c r="AD53" s="33"/>
+      <c r="AE53" s="33"/>
+      <c r="AF53" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="AG53" s="24"/>
-      <c r="AH53" s="24"/>
+      <c r="AG53" s="34"/>
+      <c r="AH53" s="34"/>
     </row>
     <row r="54" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
@@ -2168,31 +2160,31 @@
       <c r="B54" t="s">
         <v>3</v>
       </c>
-      <c r="P54" s="25"/>
-      <c r="Q54" s="25"/>
-      <c r="R54" s="25"/>
-      <c r="S54" s="24"/>
-      <c r="T54" s="24"/>
-      <c r="U54" s="24"/>
-      <c r="V54" s="26"/>
-      <c r="W54" s="26"/>
-      <c r="X54" s="26"/>
-      <c r="Y54" s="26"/>
-      <c r="Z54" s="21" t="s">
+      <c r="P54" s="30"/>
+      <c r="Q54" s="30"/>
+      <c r="R54" s="30"/>
+      <c r="S54" s="34"/>
+      <c r="T54" s="34"/>
+      <c r="U54" s="34"/>
+      <c r="V54" s="32"/>
+      <c r="W54" s="32"/>
+      <c r="X54" s="32"/>
+      <c r="Y54" s="32"/>
+      <c r="Z54" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="AA54" s="21"/>
-      <c r="AB54" s="21" t="s">
+      <c r="AA54" s="33"/>
+      <c r="AB54" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="AC54" s="21"/>
-      <c r="AD54" s="21" t="s">
+      <c r="AC54" s="33"/>
+      <c r="AD54" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="AE54" s="21"/>
-      <c r="AF54" s="24"/>
-      <c r="AG54" s="24"/>
-      <c r="AH54" s="24"/>
+      <c r="AE54" s="33"/>
+      <c r="AF54" s="34"/>
+      <c r="AG54" s="34"/>
+      <c r="AH54" s="34"/>
     </row>
     <row r="55" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
@@ -2207,40 +2199,40 @@
       <c r="D55" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="P55" s="23">
+      <c r="P55" s="31">
         <f>SUM(Z55,AD55)</f>
         <v>7</v>
       </c>
-      <c r="Q55" s="23"/>
-      <c r="R55" s="23"/>
-      <c r="S55" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="T55" s="21"/>
-      <c r="U55" s="21"/>
-      <c r="V55" s="21" t="s">
+      <c r="Q55" s="31"/>
+      <c r="R55" s="31"/>
+      <c r="S55" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="T55" s="33"/>
+      <c r="U55" s="33"/>
+      <c r="V55" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="W55" s="21"/>
-      <c r="X55" s="21"/>
-      <c r="Y55" s="21"/>
-      <c r="Z55" s="21">
+      <c r="W55" s="33"/>
+      <c r="X55" s="33"/>
+      <c r="Y55" s="33"/>
+      <c r="Z55" s="33">
         <v>4</v>
       </c>
-      <c r="AA55" s="21"/>
-      <c r="AB55" s="21">
-        <v>3</v>
-      </c>
-      <c r="AC55" s="21"/>
-      <c r="AD55" s="21">
-        <v>3</v>
-      </c>
-      <c r="AE55" s="21"/>
-      <c r="AF55" s="21" t="s">
+      <c r="AA55" s="33"/>
+      <c r="AB55" s="33">
+        <v>3</v>
+      </c>
+      <c r="AC55" s="33"/>
+      <c r="AD55" s="33">
+        <v>3</v>
+      </c>
+      <c r="AE55" s="33"/>
+      <c r="AF55" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AG55" s="21"/>
-      <c r="AH55" s="21"/>
+      <c r="AG55" s="33"/>
+      <c r="AH55" s="33"/>
       <c r="AI55" t="s">
         <v>30</v>
       </c>
@@ -2258,40 +2250,40 @@
       <c r="D56" t="s">
         <v>5</v>
       </c>
-      <c r="P56" s="23">
+      <c r="P56" s="31">
         <f t="shared" ref="P56:P59" si="0">SUM(Z56,AD56)</f>
         <v>5</v>
       </c>
-      <c r="Q56" s="23"/>
-      <c r="R56" s="23"/>
-      <c r="S56" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="T56" s="21"/>
-      <c r="U56" s="21"/>
-      <c r="V56" s="21" t="s">
+      <c r="Q56" s="31"/>
+      <c r="R56" s="31"/>
+      <c r="S56" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="T56" s="33"/>
+      <c r="U56" s="33"/>
+      <c r="V56" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="W56" s="21"/>
-      <c r="X56" s="21"/>
-      <c r="Y56" s="21"/>
-      <c r="Z56" s="21">
-        <v>2</v>
-      </c>
-      <c r="AA56" s="21"/>
-      <c r="AB56" s="21">
+      <c r="W56" s="33"/>
+      <c r="X56" s="33"/>
+      <c r="Y56" s="33"/>
+      <c r="Z56" s="33">
+        <v>2</v>
+      </c>
+      <c r="AA56" s="33"/>
+      <c r="AB56" s="33">
         <v>4</v>
       </c>
-      <c r="AC56" s="21"/>
-      <c r="AD56" s="21">
-        <v>3</v>
-      </c>
-      <c r="AE56" s="21"/>
-      <c r="AF56" s="21" t="s">
+      <c r="AC56" s="33"/>
+      <c r="AD56" s="33">
+        <v>3</v>
+      </c>
+      <c r="AE56" s="33"/>
+      <c r="AF56" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="AG56" s="21"/>
-      <c r="AH56" s="21"/>
+      <c r="AG56" s="33"/>
+      <c r="AH56" s="33"/>
       <c r="AI56" t="s">
         <v>30</v>
       </c>
@@ -2312,40 +2304,40 @@
       <c r="E57" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="P57" s="23">
+      <c r="P57" s="31">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="Q57" s="23"/>
-      <c r="R57" s="23"/>
-      <c r="S57" s="21" t="s">
+      <c r="Q57" s="31"/>
+      <c r="R57" s="31"/>
+      <c r="S57" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="T57" s="21"/>
-      <c r="U57" s="21"/>
-      <c r="V57" s="21" t="s">
+      <c r="T57" s="33"/>
+      <c r="U57" s="33"/>
+      <c r="V57" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="W57" s="21"/>
-      <c r="X57" s="21"/>
-      <c r="Y57" s="21"/>
-      <c r="Z57" s="21">
-        <v>2</v>
-      </c>
-      <c r="AA57" s="21"/>
-      <c r="AB57" s="21">
-        <v>5</v>
-      </c>
-      <c r="AC57" s="21"/>
-      <c r="AD57" s="21">
+      <c r="W57" s="33"/>
+      <c r="X57" s="33"/>
+      <c r="Y57" s="33"/>
+      <c r="Z57" s="33">
+        <v>2</v>
+      </c>
+      <c r="AA57" s="33"/>
+      <c r="AB57" s="33">
+        <v>5</v>
+      </c>
+      <c r="AC57" s="33"/>
+      <c r="AD57" s="33">
         <v>1</v>
       </c>
-      <c r="AE57" s="21"/>
-      <c r="AF57" s="21" t="s">
+      <c r="AE57" s="33"/>
+      <c r="AF57" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="AG57" s="21"/>
-      <c r="AH57" s="21"/>
+      <c r="AG57" s="33"/>
+      <c r="AH57" s="33"/>
       <c r="AI57" t="s">
         <v>30</v>
       </c>
@@ -2363,40 +2355,40 @@
       <c r="D58" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="P58" s="23">
+      <c r="P58" s="31">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="Q58" s="23"/>
-      <c r="R58" s="23"/>
-      <c r="S58" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="T58" s="21"/>
-      <c r="U58" s="21"/>
-      <c r="V58" s="21" t="s">
+      <c r="Q58" s="31"/>
+      <c r="R58" s="31"/>
+      <c r="S58" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="T58" s="33"/>
+      <c r="U58" s="33"/>
+      <c r="V58" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="W58" s="21"/>
-      <c r="X58" s="21"/>
-      <c r="Y58" s="21"/>
-      <c r="Z58" s="21">
+      <c r="W58" s="33"/>
+      <c r="X58" s="33"/>
+      <c r="Y58" s="33"/>
+      <c r="Z58" s="33">
         <v>1</v>
       </c>
-      <c r="AA58" s="21"/>
-      <c r="AB58" s="21">
+      <c r="AA58" s="33"/>
+      <c r="AB58" s="33">
         <v>4</v>
       </c>
-      <c r="AC58" s="21"/>
-      <c r="AD58" s="21">
-        <v>5</v>
-      </c>
-      <c r="AE58" s="21"/>
-      <c r="AF58" s="21" t="s">
+      <c r="AC58" s="33"/>
+      <c r="AD58" s="33">
+        <v>5</v>
+      </c>
+      <c r="AE58" s="33"/>
+      <c r="AF58" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="AG58" s="21"/>
-      <c r="AH58" s="21"/>
+      <c r="AG58" s="33"/>
+      <c r="AH58" s="33"/>
       <c r="AI58" t="s">
         <v>30</v>
       </c>
@@ -2414,40 +2406,40 @@
       <c r="D59" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="P59" s="23">
+      <c r="P59" s="31">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="Q59" s="23"/>
-      <c r="R59" s="23"/>
-      <c r="S59" s="21" t="s">
+      <c r="Q59" s="31"/>
+      <c r="R59" s="31"/>
+      <c r="S59" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="T59" s="21"/>
-      <c r="U59" s="21"/>
-      <c r="V59" s="21" t="s">
+      <c r="T59" s="33"/>
+      <c r="U59" s="33"/>
+      <c r="V59" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="W59" s="21"/>
-      <c r="X59" s="21"/>
-      <c r="Y59" s="21"/>
-      <c r="Z59" s="21">
-        <v>3</v>
-      </c>
-      <c r="AA59" s="21"/>
-      <c r="AB59" s="21">
-        <v>2</v>
-      </c>
-      <c r="AC59" s="21"/>
-      <c r="AD59" s="21">
-        <v>3</v>
-      </c>
-      <c r="AE59" s="21"/>
-      <c r="AF59" s="21" t="s">
+      <c r="W59" s="33"/>
+      <c r="X59" s="33"/>
+      <c r="Y59" s="33"/>
+      <c r="Z59" s="33">
+        <v>3</v>
+      </c>
+      <c r="AA59" s="33"/>
+      <c r="AB59" s="33">
+        <v>2</v>
+      </c>
+      <c r="AC59" s="33"/>
+      <c r="AD59" s="33">
+        <v>3</v>
+      </c>
+      <c r="AE59" s="33"/>
+      <c r="AF59" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AG59" s="21"/>
-      <c r="AH59" s="21"/>
+      <c r="AG59" s="33"/>
+      <c r="AH59" s="33"/>
       <c r="AI59" t="s">
         <v>30</v>
       </c>
@@ -2692,7 +2684,7 @@
     </row>
     <row r="83" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="85" spans="1:40" x14ac:dyDescent="0.25">
@@ -2753,10 +2745,10 @@
       <c r="S85" s="16">
         <v>18</v>
       </c>
-      <c r="T85" s="28">
+      <c r="T85" s="22">
         <v>19</v>
       </c>
-      <c r="U85" s="28">
+      <c r="U85" s="22">
         <v>20</v>
       </c>
       <c r="V85" s="16">
@@ -2789,7 +2781,7 @@
       <c r="AE85" s="16">
         <v>30</v>
       </c>
-      <c r="AF85" s="36">
+      <c r="AF85" s="28">
         <v>31</v>
       </c>
       <c r="AG85" s="16">
@@ -2839,8 +2831,8 @@
       <c r="Q86" s="16"/>
       <c r="R86" s="16"/>
       <c r="S86" s="16"/>
-      <c r="T86" s="28"/>
-      <c r="U86" s="28"/>
+      <c r="T86" s="22"/>
+      <c r="U86" s="22"/>
       <c r="V86" s="16" t="s">
         <v>7</v>
       </c>
@@ -2871,7 +2863,7 @@
       <c r="AE86" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="AF86" s="36" t="s">
+      <c r="AF86" s="28" t="s">
         <v>10</v>
       </c>
       <c r="AG86" s="16"/>
@@ -2925,8 +2917,8 @@
       <c r="Q87" s="16"/>
       <c r="R87" s="16"/>
       <c r="S87" s="16"/>
-      <c r="T87" s="28"/>
-      <c r="U87" s="28"/>
+      <c r="T87" s="22"/>
+      <c r="U87" s="22"/>
       <c r="V87" s="16"/>
       <c r="W87" s="16"/>
       <c r="X87" s="16"/>
@@ -2937,7 +2929,7 @@
       <c r="AC87" s="16"/>
       <c r="AD87" s="16"/>
       <c r="AE87" s="16"/>
-      <c r="AF87" s="36"/>
+      <c r="AF87" s="28"/>
       <c r="AG87" s="16"/>
       <c r="AH87" s="16"/>
       <c r="AI87" s="16"/>
@@ -2987,8 +2979,8 @@
       <c r="Q88" s="16"/>
       <c r="R88" s="16"/>
       <c r="S88" s="16"/>
-      <c r="T88" s="28"/>
-      <c r="U88" s="28"/>
+      <c r="T88" s="22"/>
+      <c r="U88" s="22"/>
       <c r="V88" s="16"/>
       <c r="W88" s="16"/>
       <c r="X88" s="16"/>
@@ -2999,7 +2991,7 @@
       <c r="AC88" s="16"/>
       <c r="AD88" s="16"/>
       <c r="AE88" s="16"/>
-      <c r="AF88" s="36"/>
+      <c r="AF88" s="28"/>
       <c r="AG88" s="16"/>
       <c r="AH88" s="16"/>
       <c r="AI88" s="16"/>
@@ -3047,10 +3039,10 @@
       <c r="S89" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="T89" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="U89" s="28" t="s">
+      <c r="T89" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="U89" s="22" t="s">
         <v>7</v>
       </c>
       <c r="V89" s="16" t="s">
@@ -3065,7 +3057,7 @@
       <c r="AC89" s="16"/>
       <c r="AD89" s="16"/>
       <c r="AE89" s="16"/>
-      <c r="AF89" s="36"/>
+      <c r="AF89" s="28"/>
       <c r="AG89" s="16"/>
       <c r="AH89" s="16"/>
       <c r="AI89" s="16"/>
@@ -3117,8 +3109,8 @@
       </c>
       <c r="R90" s="16"/>
       <c r="S90" s="16"/>
-      <c r="T90" s="28"/>
-      <c r="U90" s="28"/>
+      <c r="T90" s="22"/>
+      <c r="U90" s="22"/>
       <c r="V90" s="16"/>
       <c r="W90" s="16"/>
       <c r="X90" s="16"/>
@@ -3129,7 +3121,7 @@
       <c r="AC90" s="16"/>
       <c r="AD90" s="16"/>
       <c r="AE90" s="16"/>
-      <c r="AF90" s="36"/>
+      <c r="AF90" s="28"/>
       <c r="AG90" s="16"/>
       <c r="AH90" s="16"/>
       <c r="AI90" s="16"/>
@@ -3166,35 +3158,35 @@
       <c r="C93" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="Q93" s="25" t="s">
+      <c r="Q93" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="R93" s="25"/>
-      <c r="S93" s="25"/>
-      <c r="T93" s="24" t="s">
+      <c r="R93" s="30"/>
+      <c r="S93" s="30"/>
+      <c r="T93" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="U93" s="24"/>
-      <c r="V93" s="24"/>
-      <c r="W93" s="26" t="s">
+      <c r="U93" s="34"/>
+      <c r="V93" s="34"/>
+      <c r="W93" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="X93" s="26"/>
-      <c r="Y93" s="26"/>
-      <c r="Z93" s="26"/>
-      <c r="AA93" s="21" t="s">
+      <c r="X93" s="32"/>
+      <c r="Y93" s="32"/>
+      <c r="Z93" s="32"/>
+      <c r="AA93" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="AB93" s="21"/>
-      <c r="AC93" s="21"/>
-      <c r="AD93" s="21"/>
-      <c r="AE93" s="21"/>
-      <c r="AF93" s="21"/>
-      <c r="AG93" s="24" t="s">
+      <c r="AB93" s="33"/>
+      <c r="AC93" s="33"/>
+      <c r="AD93" s="33"/>
+      <c r="AE93" s="33"/>
+      <c r="AF93" s="33"/>
+      <c r="AG93" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="AH93" s="24"/>
-      <c r="AI93" s="24"/>
+      <c r="AH93" s="34"/>
+      <c r="AI93" s="34"/>
     </row>
     <row r="94" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
@@ -3203,31 +3195,31 @@
       <c r="B94" t="s">
         <v>2</v>
       </c>
-      <c r="Q94" s="25"/>
-      <c r="R94" s="25"/>
-      <c r="S94" s="25"/>
-      <c r="T94" s="24"/>
-      <c r="U94" s="24"/>
-      <c r="V94" s="24"/>
-      <c r="W94" s="26"/>
-      <c r="X94" s="26"/>
-      <c r="Y94" s="26"/>
-      <c r="Z94" s="26"/>
-      <c r="AA94" s="21" t="s">
+      <c r="Q94" s="30"/>
+      <c r="R94" s="30"/>
+      <c r="S94" s="30"/>
+      <c r="T94" s="34"/>
+      <c r="U94" s="34"/>
+      <c r="V94" s="34"/>
+      <c r="W94" s="32"/>
+      <c r="X94" s="32"/>
+      <c r="Y94" s="32"/>
+      <c r="Z94" s="32"/>
+      <c r="AA94" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="AB94" s="21"/>
-      <c r="AC94" s="21" t="s">
+      <c r="AB94" s="33"/>
+      <c r="AC94" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="AD94" s="21"/>
-      <c r="AE94" s="21" t="s">
+      <c r="AD94" s="33"/>
+      <c r="AE94" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="AF94" s="21"/>
-      <c r="AG94" s="24"/>
-      <c r="AH94" s="24"/>
-      <c r="AI94" s="24"/>
+      <c r="AF94" s="33"/>
+      <c r="AG94" s="34"/>
+      <c r="AH94" s="34"/>
+      <c r="AI94" s="34"/>
     </row>
     <row r="95" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
@@ -3242,40 +3234,40 @@
       <c r="D95" t="s">
         <v>2</v>
       </c>
-      <c r="Q95" s="23">
+      <c r="Q95" s="31">
         <f>SUM(AA95,AE95)</f>
         <v>7</v>
       </c>
-      <c r="R95" s="23"/>
-      <c r="S95" s="23"/>
-      <c r="T95" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="U95" s="21"/>
-      <c r="V95" s="21"/>
-      <c r="W95" s="21" t="s">
+      <c r="R95" s="31"/>
+      <c r="S95" s="31"/>
+      <c r="T95" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="U95" s="33"/>
+      <c r="V95" s="33"/>
+      <c r="W95" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="X95" s="21"/>
-      <c r="Y95" s="21"/>
-      <c r="Z95" s="21"/>
-      <c r="AA95" s="21">
+      <c r="X95" s="33"/>
+      <c r="Y95" s="33"/>
+      <c r="Z95" s="33"/>
+      <c r="AA95" s="33">
         <v>4</v>
       </c>
-      <c r="AB95" s="21"/>
-      <c r="AC95" s="21">
-        <v>3</v>
-      </c>
-      <c r="AD95" s="21"/>
-      <c r="AE95" s="21">
-        <v>3</v>
-      </c>
-      <c r="AF95" s="21"/>
-      <c r="AG95" s="21" t="s">
+      <c r="AB95" s="33"/>
+      <c r="AC95" s="33">
+        <v>3</v>
+      </c>
+      <c r="AD95" s="33"/>
+      <c r="AE95" s="33">
+        <v>3</v>
+      </c>
+      <c r="AF95" s="33"/>
+      <c r="AG95" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AH95" s="21"/>
-      <c r="AI95" s="21"/>
+      <c r="AH95" s="33"/>
+      <c r="AI95" s="33"/>
     </row>
     <row r="96" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
@@ -3287,46 +3279,46 @@
       <c r="C96" t="s">
         <v>2</v>
       </c>
-      <c r="Q96" s="23">
+      <c r="Q96" s="31">
         <f t="shared" ref="Q96:Q99" si="1">SUM(AA96,AE96)</f>
         <v>5</v>
       </c>
-      <c r="R96" s="23"/>
-      <c r="S96" s="23"/>
-      <c r="T96" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="U96" s="21"/>
-      <c r="V96" s="21"/>
-      <c r="W96" s="21" t="s">
+      <c r="R96" s="31"/>
+      <c r="S96" s="31"/>
+      <c r="T96" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="U96" s="33"/>
+      <c r="V96" s="33"/>
+      <c r="W96" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="X96" s="21"/>
-      <c r="Y96" s="21"/>
-      <c r="Z96" s="21"/>
-      <c r="AA96" s="21">
-        <v>2</v>
-      </c>
-      <c r="AB96" s="21"/>
-      <c r="AC96" s="21">
+      <c r="X96" s="33"/>
+      <c r="Y96" s="33"/>
+      <c r="Z96" s="33"/>
+      <c r="AA96" s="33">
+        <v>2</v>
+      </c>
+      <c r="AB96" s="33"/>
+      <c r="AC96" s="33">
         <v>4</v>
       </c>
-      <c r="AD96" s="21"/>
-      <c r="AE96" s="21">
-        <v>3</v>
-      </c>
-      <c r="AF96" s="21"/>
-      <c r="AG96" s="21" t="s">
+      <c r="AD96" s="33"/>
+      <c r="AE96" s="33">
+        <v>3</v>
+      </c>
+      <c r="AF96" s="33"/>
+      <c r="AG96" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="AH96" s="21"/>
-      <c r="AI96" s="21"/>
+      <c r="AH96" s="33"/>
+      <c r="AI96" s="33"/>
     </row>
     <row r="97" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A97" s="5">
         <v>5</v>
       </c>
-      <c r="B97" s="32" t="s">
+      <c r="B97" s="24" t="s">
         <v>5</v>
       </c>
       <c r="C97" s="2" t="s">
@@ -3335,40 +3327,40 @@
       <c r="D97" t="s">
         <v>2</v>
       </c>
-      <c r="Q97" s="23">
+      <c r="Q97" s="31">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="R97" s="23"/>
-      <c r="S97" s="23"/>
-      <c r="T97" s="21" t="s">
+      <c r="R97" s="31"/>
+      <c r="S97" s="31"/>
+      <c r="T97" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="U97" s="21"/>
-      <c r="V97" s="21"/>
-      <c r="W97" s="21" t="s">
+      <c r="U97" s="33"/>
+      <c r="V97" s="33"/>
+      <c r="W97" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="X97" s="21"/>
-      <c r="Y97" s="21"/>
-      <c r="Z97" s="21"/>
-      <c r="AA97" s="21">
-        <v>2</v>
-      </c>
-      <c r="AB97" s="21"/>
-      <c r="AC97" s="21">
-        <v>5</v>
-      </c>
-      <c r="AD97" s="21"/>
-      <c r="AE97" s="21">
+      <c r="X97" s="33"/>
+      <c r="Y97" s="33"/>
+      <c r="Z97" s="33"/>
+      <c r="AA97" s="33">
+        <v>2</v>
+      </c>
+      <c r="AB97" s="33"/>
+      <c r="AC97" s="33">
+        <v>5</v>
+      </c>
+      <c r="AD97" s="33"/>
+      <c r="AE97" s="33">
         <v>1</v>
       </c>
-      <c r="AF97" s="21"/>
-      <c r="AG97" s="21" t="s">
+      <c r="AF97" s="33"/>
+      <c r="AG97" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="AH97" s="21"/>
-      <c r="AI97" s="21"/>
+      <c r="AH97" s="33"/>
+      <c r="AI97" s="33"/>
     </row>
     <row r="98" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
@@ -3380,40 +3372,40 @@
       <c r="C98" t="s">
         <v>2</v>
       </c>
-      <c r="Q98" s="23">
+      <c r="Q98" s="31">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="R98" s="23"/>
-      <c r="S98" s="23"/>
-      <c r="T98" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="U98" s="21"/>
-      <c r="V98" s="21"/>
-      <c r="W98" s="21" t="s">
+      <c r="R98" s="31"/>
+      <c r="S98" s="31"/>
+      <c r="T98" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="U98" s="33"/>
+      <c r="V98" s="33"/>
+      <c r="W98" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="X98" s="21"/>
-      <c r="Y98" s="21"/>
-      <c r="Z98" s="21"/>
-      <c r="AA98" s="21">
+      <c r="X98" s="33"/>
+      <c r="Y98" s="33"/>
+      <c r="Z98" s="33"/>
+      <c r="AA98" s="33">
         <v>1</v>
       </c>
-      <c r="AB98" s="21"/>
-      <c r="AC98" s="21">
+      <c r="AB98" s="33"/>
+      <c r="AC98" s="33">
         <v>4</v>
       </c>
-      <c r="AD98" s="21"/>
-      <c r="AE98" s="21">
-        <v>5</v>
-      </c>
-      <c r="AF98" s="21"/>
-      <c r="AG98" s="21" t="s">
+      <c r="AD98" s="33"/>
+      <c r="AE98" s="33">
+        <v>5</v>
+      </c>
+      <c r="AF98" s="33"/>
+      <c r="AG98" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="AH98" s="21"/>
-      <c r="AI98" s="21"/>
+      <c r="AH98" s="33"/>
+      <c r="AI98" s="33"/>
     </row>
     <row r="99" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
@@ -3425,40 +3417,40 @@
       <c r="C99" t="s">
         <v>2</v>
       </c>
-      <c r="Q99" s="23">
+      <c r="Q99" s="31">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="R99" s="23"/>
-      <c r="S99" s="23"/>
-      <c r="T99" s="21" t="s">
+      <c r="R99" s="31"/>
+      <c r="S99" s="31"/>
+      <c r="T99" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="U99" s="21"/>
-      <c r="V99" s="21"/>
-      <c r="W99" s="21" t="s">
+      <c r="U99" s="33"/>
+      <c r="V99" s="33"/>
+      <c r="W99" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="X99" s="21"/>
-      <c r="Y99" s="21"/>
-      <c r="Z99" s="21"/>
-      <c r="AA99" s="21">
-        <v>3</v>
-      </c>
-      <c r="AB99" s="21"/>
-      <c r="AC99" s="21">
-        <v>2</v>
-      </c>
-      <c r="AD99" s="21"/>
-      <c r="AE99" s="21">
-        <v>3</v>
-      </c>
-      <c r="AF99" s="21"/>
-      <c r="AG99" s="21" t="s">
+      <c r="X99" s="33"/>
+      <c r="Y99" s="33"/>
+      <c r="Z99" s="33"/>
+      <c r="AA99" s="33">
+        <v>3</v>
+      </c>
+      <c r="AB99" s="33"/>
+      <c r="AC99" s="33">
+        <v>2</v>
+      </c>
+      <c r="AD99" s="33"/>
+      <c r="AE99" s="33">
+        <v>3</v>
+      </c>
+      <c r="AF99" s="33"/>
+      <c r="AG99" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AH99" s="21"/>
-      <c r="AI99" s="21"/>
+      <c r="AH99" s="33"/>
+      <c r="AI99" s="33"/>
     </row>
     <row r="100" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
@@ -3475,140 +3467,140 @@
       <c r="A101" s="5">
         <v>9</v>
       </c>
-      <c r="B101" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="C101" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="D101" s="33"/>
-      <c r="E101" s="33"/>
-      <c r="F101" s="33"/>
-      <c r="Q101" s="25" t="s">
+      <c r="B101" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C101" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D101" s="25"/>
+      <c r="E101" s="25"/>
+      <c r="F101" s="25"/>
+      <c r="Q101" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="R101" s="25"/>
-      <c r="S101" s="25"/>
-      <c r="T101" s="24" t="s">
+      <c r="R101" s="30"/>
+      <c r="S101" s="30"/>
+      <c r="T101" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="U101" s="24"/>
-      <c r="V101" s="24"/>
-      <c r="W101" s="26" t="s">
+      <c r="U101" s="34"/>
+      <c r="V101" s="34"/>
+      <c r="W101" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="X101" s="26"/>
-      <c r="Y101" s="26"/>
-      <c r="Z101" s="26"/>
-      <c r="AA101" s="21" t="s">
+      <c r="X101" s="32"/>
+      <c r="Y101" s="32"/>
+      <c r="Z101" s="32"/>
+      <c r="AA101" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="AB101" s="21"/>
-      <c r="AC101" s="21"/>
-      <c r="AD101" s="21"/>
-      <c r="AE101" s="21"/>
-      <c r="AF101" s="21"/>
-      <c r="AG101" s="24" t="s">
+      <c r="AB101" s="33"/>
+      <c r="AC101" s="33"/>
+      <c r="AD101" s="33"/>
+      <c r="AE101" s="33"/>
+      <c r="AF101" s="33"/>
+      <c r="AG101" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="AH101" s="24"/>
-      <c r="AI101" s="24"/>
+      <c r="AH101" s="34"/>
+      <c r="AI101" s="34"/>
     </row>
     <row r="102" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <v>10</v>
       </c>
-      <c r="B102" s="33" t="s">
+      <c r="B102" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C102" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D102" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="E102" s="33"/>
-      <c r="F102" s="33"/>
-      <c r="Q102" s="25"/>
-      <c r="R102" s="25"/>
-      <c r="S102" s="25"/>
-      <c r="T102" s="24"/>
-      <c r="U102" s="24"/>
-      <c r="V102" s="24"/>
-      <c r="W102" s="26"/>
-      <c r="X102" s="26"/>
-      <c r="Y102" s="26"/>
-      <c r="Z102" s="26"/>
-      <c r="AA102" s="21" t="s">
+      <c r="C102" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D102" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E102" s="25"/>
+      <c r="F102" s="25"/>
+      <c r="Q102" s="30"/>
+      <c r="R102" s="30"/>
+      <c r="S102" s="30"/>
+      <c r="T102" s="34"/>
+      <c r="U102" s="34"/>
+      <c r="V102" s="34"/>
+      <c r="W102" s="32"/>
+      <c r="X102" s="32"/>
+      <c r="Y102" s="32"/>
+      <c r="Z102" s="32"/>
+      <c r="AA102" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="AB102" s="21"/>
-      <c r="AC102" s="21" t="s">
+      <c r="AB102" s="33"/>
+      <c r="AC102" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="AD102" s="21"/>
-      <c r="AE102" s="21" t="s">
+      <c r="AD102" s="33"/>
+      <c r="AE102" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="AF102" s="21"/>
-      <c r="AG102" s="24"/>
-      <c r="AH102" s="24"/>
-      <c r="AI102" s="24"/>
+      <c r="AF102" s="33"/>
+      <c r="AG102" s="34"/>
+      <c r="AH102" s="34"/>
+      <c r="AI102" s="34"/>
     </row>
     <row r="103" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
         <v>11</v>
       </c>
-      <c r="B103" s="33" t="s">
+      <c r="B103" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C103" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D103" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="E103" s="33"/>
+      <c r="C103" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D103" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E103" s="25"/>
       <c r="F103" s="19"/>
-      <c r="Q103" s="23">
+      <c r="Q103" s="31">
         <v>0</v>
       </c>
-      <c r="R103" s="23"/>
-      <c r="S103" s="23"/>
-      <c r="T103" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="U103" s="21"/>
-      <c r="V103" s="21"/>
-      <c r="W103" s="29" t="s">
+      <c r="R103" s="31"/>
+      <c r="S103" s="31"/>
+      <c r="T103" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="U103" s="33"/>
+      <c r="V103" s="33"/>
+      <c r="W103" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="X103" s="29"/>
-      <c r="Y103" s="29"/>
-      <c r="Z103" s="29"/>
-      <c r="AA103" s="29">
+      <c r="X103" s="36"/>
+      <c r="Y103" s="36"/>
+      <c r="Z103" s="36"/>
+      <c r="AA103" s="36">
         <v>4</v>
       </c>
-      <c r="AB103" s="29"/>
-      <c r="AC103" s="29">
-        <v>3</v>
-      </c>
-      <c r="AD103" s="29"/>
-      <c r="AE103" s="29">
-        <v>3</v>
-      </c>
-      <c r="AF103" s="29"/>
-      <c r="AG103" s="21" t="s">
+      <c r="AB103" s="36"/>
+      <c r="AC103" s="36">
+        <v>3</v>
+      </c>
+      <c r="AD103" s="36"/>
+      <c r="AE103" s="36">
+        <v>3</v>
+      </c>
+      <c r="AF103" s="36"/>
+      <c r="AG103" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AH103" s="21"/>
-      <c r="AI103" s="21"/>
+      <c r="AH103" s="33"/>
+      <c r="AI103" s="33"/>
     </row>
     <row r="104" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <v>12</v>
       </c>
-      <c r="B104" s="32" t="s">
+      <c r="B104" s="24" t="s">
         <v>4</v>
       </c>
       <c r="C104" s="19" t="s">
@@ -3621,45 +3613,45 @@
         <v>2</v>
       </c>
       <c r="F104" s="19"/>
-      <c r="Q104" s="30">
+      <c r="Q104" s="37">
         <v>0</v>
       </c>
-      <c r="R104" s="30"/>
-      <c r="S104" s="30"/>
-      <c r="T104" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="U104" s="21"/>
-      <c r="V104" s="21"/>
-      <c r="W104" s="29" t="s">
+      <c r="R104" s="37"/>
+      <c r="S104" s="37"/>
+      <c r="T104" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="U104" s="33"/>
+      <c r="V104" s="33"/>
+      <c r="W104" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="X104" s="29"/>
-      <c r="Y104" s="29"/>
-      <c r="Z104" s="29"/>
-      <c r="AA104" s="29">
-        <v>2</v>
-      </c>
-      <c r="AB104" s="29"/>
-      <c r="AC104" s="29">
+      <c r="X104" s="36"/>
+      <c r="Y104" s="36"/>
+      <c r="Z104" s="36"/>
+      <c r="AA104" s="36">
+        <v>2</v>
+      </c>
+      <c r="AB104" s="36"/>
+      <c r="AC104" s="36">
         <v>4</v>
       </c>
-      <c r="AD104" s="29"/>
-      <c r="AE104" s="29">
-        <v>3</v>
-      </c>
-      <c r="AF104" s="29"/>
-      <c r="AG104" s="21" t="s">
+      <c r="AD104" s="36"/>
+      <c r="AE104" s="36">
+        <v>3</v>
+      </c>
+      <c r="AF104" s="36"/>
+      <c r="AG104" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="AH104" s="21"/>
-      <c r="AI104" s="21"/>
+      <c r="AH104" s="33"/>
+      <c r="AI104" s="33"/>
     </row>
     <row r="105" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
         <v>13</v>
       </c>
-      <c r="B105" s="32" t="s">
+      <c r="B105" s="24" t="s">
         <v>6</v>
       </c>
       <c r="C105" s="19" t="s">
@@ -3670,39 +3662,39 @@
       </c>
       <c r="E105" s="19"/>
       <c r="F105" s="19"/>
-      <c r="Q105" s="30">
+      <c r="Q105" s="37">
         <v>0</v>
       </c>
-      <c r="R105" s="30"/>
-      <c r="S105" s="30"/>
-      <c r="T105" s="21" t="s">
+      <c r="R105" s="37"/>
+      <c r="S105" s="37"/>
+      <c r="T105" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="U105" s="21"/>
-      <c r="V105" s="21"/>
-      <c r="W105" s="29" t="s">
+      <c r="U105" s="33"/>
+      <c r="V105" s="33"/>
+      <c r="W105" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="X105" s="29"/>
-      <c r="Y105" s="29"/>
-      <c r="Z105" s="29"/>
-      <c r="AA105" s="29">
-        <v>2</v>
-      </c>
-      <c r="AB105" s="29"/>
-      <c r="AC105" s="29">
-        <v>5</v>
-      </c>
-      <c r="AD105" s="29"/>
-      <c r="AE105" s="29">
+      <c r="X105" s="36"/>
+      <c r="Y105" s="36"/>
+      <c r="Z105" s="36"/>
+      <c r="AA105" s="36">
+        <v>2</v>
+      </c>
+      <c r="AB105" s="36"/>
+      <c r="AC105" s="36">
+        <v>5</v>
+      </c>
+      <c r="AD105" s="36"/>
+      <c r="AE105" s="36">
         <v>1</v>
       </c>
-      <c r="AF105" s="29"/>
-      <c r="AG105" s="21" t="s">
+      <c r="AF105" s="36"/>
+      <c r="AG105" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="AH105" s="21"/>
-      <c r="AI105" s="21"/>
+      <c r="AH105" s="33"/>
+      <c r="AI105" s="33"/>
     </row>
     <row r="106" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
@@ -3717,39 +3709,39 @@
       <c r="D106" s="19"/>
       <c r="E106" s="19"/>
       <c r="F106" s="19"/>
-      <c r="Q106" s="30">
+      <c r="Q106" s="37">
         <v>0</v>
       </c>
-      <c r="R106" s="30"/>
-      <c r="S106" s="30"/>
-      <c r="T106" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="U106" s="21"/>
-      <c r="V106" s="21"/>
-      <c r="W106" s="29" t="s">
+      <c r="R106" s="37"/>
+      <c r="S106" s="37"/>
+      <c r="T106" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="U106" s="33"/>
+      <c r="V106" s="33"/>
+      <c r="W106" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="X106" s="29"/>
-      <c r="Y106" s="29"/>
-      <c r="Z106" s="29"/>
-      <c r="AA106" s="29">
+      <c r="X106" s="36"/>
+      <c r="Y106" s="36"/>
+      <c r="Z106" s="36"/>
+      <c r="AA106" s="36">
         <v>1</v>
       </c>
-      <c r="AB106" s="29"/>
-      <c r="AC106" s="29">
+      <c r="AB106" s="36"/>
+      <c r="AC106" s="36">
         <v>4</v>
       </c>
-      <c r="AD106" s="29"/>
-      <c r="AE106" s="29">
-        <v>5</v>
-      </c>
-      <c r="AF106" s="29"/>
-      <c r="AG106" s="21" t="s">
+      <c r="AD106" s="36"/>
+      <c r="AE106" s="36">
+        <v>5</v>
+      </c>
+      <c r="AF106" s="36"/>
+      <c r="AG106" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="AH106" s="21"/>
-      <c r="AI106" s="21"/>
+      <c r="AH106" s="33"/>
+      <c r="AI106" s="33"/>
     </row>
     <row r="107" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A107" s="5">
@@ -3764,45 +3756,45 @@
       <c r="D107" s="19"/>
       <c r="E107" s="19"/>
       <c r="F107" s="19"/>
-      <c r="Q107" s="30">
+      <c r="Q107" s="37">
         <v>0</v>
       </c>
-      <c r="R107" s="30"/>
-      <c r="S107" s="30"/>
-      <c r="T107" s="21" t="s">
+      <c r="R107" s="37"/>
+      <c r="S107" s="37"/>
+      <c r="T107" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="U107" s="21"/>
-      <c r="V107" s="21"/>
-      <c r="W107" s="29" t="s">
+      <c r="U107" s="33"/>
+      <c r="V107" s="33"/>
+      <c r="W107" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="X107" s="29"/>
-      <c r="Y107" s="29"/>
-      <c r="Z107" s="29"/>
-      <c r="AA107" s="29">
-        <v>3</v>
-      </c>
-      <c r="AB107" s="29"/>
-      <c r="AC107" s="29">
-        <v>2</v>
-      </c>
-      <c r="AD107" s="29"/>
-      <c r="AE107" s="29">
-        <v>3</v>
-      </c>
-      <c r="AF107" s="29"/>
-      <c r="AG107" s="21" t="s">
+      <c r="X107" s="36"/>
+      <c r="Y107" s="36"/>
+      <c r="Z107" s="36"/>
+      <c r="AA107" s="36">
+        <v>3</v>
+      </c>
+      <c r="AB107" s="36"/>
+      <c r="AC107" s="36">
+        <v>2</v>
+      </c>
+      <c r="AD107" s="36"/>
+      <c r="AE107" s="36">
+        <v>3</v>
+      </c>
+      <c r="AF107" s="36"/>
+      <c r="AG107" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AH107" s="21"/>
-      <c r="AI107" s="21"/>
+      <c r="AH107" s="33"/>
+      <c r="AI107" s="33"/>
     </row>
     <row r="108" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
         <v>16</v>
       </c>
-      <c r="B108" s="32" t="s">
+      <c r="B108" s="24" t="s">
         <v>5</v>
       </c>
       <c r="C108" s="19" t="s">
@@ -3832,10 +3824,10 @@
       <c r="B110" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C110" s="33"/>
-      <c r="D110" s="33"/>
-      <c r="E110" s="33"/>
-      <c r="F110" s="33"/>
+      <c r="C110" s="25"/>
+      <c r="D110" s="25"/>
+      <c r="E110" s="25"/>
+      <c r="F110" s="25"/>
     </row>
     <row r="111" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A111" s="5">
@@ -3865,10 +3857,10 @@
       <c r="A113" s="5">
         <v>21</v>
       </c>
-      <c r="B113" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="C113" s="31"/>
+      <c r="B113" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C113" s="23"/>
       <c r="D113" s="10"/>
       <c r="E113" s="10"/>
       <c r="F113" s="10"/>
@@ -3943,7 +3935,7 @@
       <c r="A120" s="5">
         <v>28</v>
       </c>
-      <c r="B120" s="32" t="s">
+      <c r="B120" s="24" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3969,13 +3961,156 @@
       <c r="A124" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B124" s="35">
+      <c r="B124" s="27">
         <f>A123</f>
         <v>31</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="168">
+  <mergeCells count="167">
+    <mergeCell ref="AG107:AI107"/>
+    <mergeCell ref="Q107:S107"/>
+    <mergeCell ref="T107:V107"/>
+    <mergeCell ref="W107:Z107"/>
+    <mergeCell ref="AA107:AB107"/>
+    <mergeCell ref="AC107:AD107"/>
+    <mergeCell ref="AE107:AF107"/>
+    <mergeCell ref="AG105:AI105"/>
+    <mergeCell ref="Q106:S106"/>
+    <mergeCell ref="T106:V106"/>
+    <mergeCell ref="W106:Z106"/>
+    <mergeCell ref="AA106:AB106"/>
+    <mergeCell ref="AC106:AD106"/>
+    <mergeCell ref="AE106:AF106"/>
+    <mergeCell ref="AG106:AI106"/>
+    <mergeCell ref="Q105:S105"/>
+    <mergeCell ref="T105:V105"/>
+    <mergeCell ref="W105:Z105"/>
+    <mergeCell ref="AA105:AB105"/>
+    <mergeCell ref="AC105:AD105"/>
+    <mergeCell ref="AE105:AF105"/>
+    <mergeCell ref="AG103:AI103"/>
+    <mergeCell ref="Q104:S104"/>
+    <mergeCell ref="T104:V104"/>
+    <mergeCell ref="W104:Z104"/>
+    <mergeCell ref="AA104:AB104"/>
+    <mergeCell ref="AC104:AD104"/>
+    <mergeCell ref="AE104:AF104"/>
+    <mergeCell ref="AG104:AI104"/>
+    <mergeCell ref="AG101:AI102"/>
+    <mergeCell ref="AA102:AB102"/>
+    <mergeCell ref="AC102:AD102"/>
+    <mergeCell ref="AE102:AF102"/>
+    <mergeCell ref="Q103:S103"/>
+    <mergeCell ref="T103:V103"/>
+    <mergeCell ref="W103:Z103"/>
+    <mergeCell ref="AA103:AB103"/>
+    <mergeCell ref="AC103:AD103"/>
+    <mergeCell ref="AE103:AF103"/>
+    <mergeCell ref="P58:R58"/>
+    <mergeCell ref="P59:R59"/>
+    <mergeCell ref="Q101:S102"/>
+    <mergeCell ref="T101:V102"/>
+    <mergeCell ref="W101:Z102"/>
+    <mergeCell ref="AA101:AF101"/>
+    <mergeCell ref="AD59:AE59"/>
+    <mergeCell ref="P56:R56"/>
+    <mergeCell ref="P57:R57"/>
+    <mergeCell ref="S59:U59"/>
+    <mergeCell ref="V59:Y59"/>
+    <mergeCell ref="Z59:AA59"/>
+    <mergeCell ref="AB59:AC59"/>
+    <mergeCell ref="S56:U56"/>
+    <mergeCell ref="V56:Y56"/>
+    <mergeCell ref="Z56:AA56"/>
+    <mergeCell ref="AB56:AC56"/>
+    <mergeCell ref="AF59:AH59"/>
+    <mergeCell ref="S58:U58"/>
+    <mergeCell ref="V58:Y58"/>
+    <mergeCell ref="Z58:AA58"/>
+    <mergeCell ref="AB58:AC58"/>
+    <mergeCell ref="AD58:AE58"/>
+    <mergeCell ref="AF58:AH58"/>
+    <mergeCell ref="S57:U57"/>
+    <mergeCell ref="V57:Y57"/>
+    <mergeCell ref="Z57:AA57"/>
+    <mergeCell ref="AB57:AC57"/>
+    <mergeCell ref="AD57:AE57"/>
+    <mergeCell ref="AF57:AH57"/>
+    <mergeCell ref="AF55:AH55"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="S53:U54"/>
+    <mergeCell ref="V53:Y54"/>
+    <mergeCell ref="Z53:AE53"/>
+    <mergeCell ref="AF53:AH54"/>
+    <mergeCell ref="Z54:AA54"/>
+    <mergeCell ref="AB54:AC54"/>
+    <mergeCell ref="AD54:AE54"/>
+    <mergeCell ref="V17:Y17"/>
+    <mergeCell ref="P52:R52"/>
+    <mergeCell ref="P53:R54"/>
+    <mergeCell ref="P55:R55"/>
+    <mergeCell ref="Z11:AE11"/>
+    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="AD13:AE13"/>
+    <mergeCell ref="AD14:AE14"/>
+    <mergeCell ref="AD15:AE15"/>
+    <mergeCell ref="AD16:AE16"/>
+    <mergeCell ref="AD17:AE17"/>
+    <mergeCell ref="P11:R12"/>
+    <mergeCell ref="P13:R13"/>
+    <mergeCell ref="P14:R14"/>
+    <mergeCell ref="P15:R15"/>
+    <mergeCell ref="Z14:AA14"/>
+    <mergeCell ref="Z15:AA15"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="Z17:AA17"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AB15:AC15"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="V11:Y12"/>
+    <mergeCell ref="S11:U12"/>
+    <mergeCell ref="V13:Y13"/>
+    <mergeCell ref="V14:Y14"/>
+    <mergeCell ref="T96:V96"/>
+    <mergeCell ref="T97:V97"/>
+    <mergeCell ref="AC97:AD97"/>
+    <mergeCell ref="AE97:AF97"/>
+    <mergeCell ref="AG97:AI97"/>
+    <mergeCell ref="T93:V94"/>
+    <mergeCell ref="T95:V95"/>
+    <mergeCell ref="Z12:AA12"/>
+    <mergeCell ref="AB12:AC12"/>
+    <mergeCell ref="S13:U13"/>
+    <mergeCell ref="S14:U14"/>
+    <mergeCell ref="S15:U15"/>
+    <mergeCell ref="S16:U16"/>
+    <mergeCell ref="S17:U17"/>
+    <mergeCell ref="AD12:AE12"/>
+    <mergeCell ref="V15:Y15"/>
+    <mergeCell ref="V16:Y16"/>
+    <mergeCell ref="AD56:AE56"/>
+    <mergeCell ref="AF56:AH56"/>
+    <mergeCell ref="S55:U55"/>
+    <mergeCell ref="V55:Y55"/>
+    <mergeCell ref="Z55:AA55"/>
+    <mergeCell ref="AB55:AC55"/>
+    <mergeCell ref="AD55:AE55"/>
+    <mergeCell ref="T98:V98"/>
+    <mergeCell ref="T99:V99"/>
+    <mergeCell ref="W98:Z98"/>
+    <mergeCell ref="AA98:AB98"/>
+    <mergeCell ref="AC98:AD98"/>
+    <mergeCell ref="AE98:AF98"/>
+    <mergeCell ref="AG98:AI98"/>
+    <mergeCell ref="W99:Z99"/>
+    <mergeCell ref="AA99:AB99"/>
+    <mergeCell ref="AC99:AD99"/>
+    <mergeCell ref="AE99:AF99"/>
+    <mergeCell ref="AG99:AI99"/>
     <mergeCell ref="Q93:S94"/>
     <mergeCell ref="Q95:S95"/>
     <mergeCell ref="Q96:S96"/>
@@ -4000,150 +4135,6 @@
     <mergeCell ref="AG96:AI96"/>
     <mergeCell ref="W97:Z97"/>
     <mergeCell ref="AA97:AB97"/>
-    <mergeCell ref="T98:V98"/>
-    <mergeCell ref="T99:V99"/>
-    <mergeCell ref="W98:Z98"/>
-    <mergeCell ref="AA98:AB98"/>
-    <mergeCell ref="AC98:AD98"/>
-    <mergeCell ref="AE98:AF98"/>
-    <mergeCell ref="AG98:AI98"/>
-    <mergeCell ref="W99:Z99"/>
-    <mergeCell ref="AA99:AB99"/>
-    <mergeCell ref="AC99:AD99"/>
-    <mergeCell ref="AE99:AF99"/>
-    <mergeCell ref="AG99:AI99"/>
-    <mergeCell ref="T96:V96"/>
-    <mergeCell ref="T97:V97"/>
-    <mergeCell ref="AC97:AD97"/>
-    <mergeCell ref="AE97:AF97"/>
-    <mergeCell ref="AG97:AI97"/>
-    <mergeCell ref="T93:V94"/>
-    <mergeCell ref="T95:V95"/>
-    <mergeCell ref="Z12:AA12"/>
-    <mergeCell ref="AB12:AC12"/>
-    <mergeCell ref="S13:U13"/>
-    <mergeCell ref="S14:U14"/>
-    <mergeCell ref="S15:U15"/>
-    <mergeCell ref="S16:U16"/>
-    <mergeCell ref="S17:U17"/>
-    <mergeCell ref="AD12:AE12"/>
-    <mergeCell ref="Z11:AE11"/>
-    <mergeCell ref="Z13:AA13"/>
-    <mergeCell ref="AD13:AE13"/>
-    <mergeCell ref="AD14:AE14"/>
-    <mergeCell ref="AD15:AE15"/>
-    <mergeCell ref="AD16:AE16"/>
-    <mergeCell ref="AD17:AE17"/>
-    <mergeCell ref="P11:R12"/>
-    <mergeCell ref="P13:R13"/>
-    <mergeCell ref="P14:R14"/>
-    <mergeCell ref="P15:R15"/>
-    <mergeCell ref="Z14:AA14"/>
-    <mergeCell ref="Z15:AA15"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="Z17:AA17"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AB15:AC15"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AB17:AC17"/>
-    <mergeCell ref="V11:Y12"/>
-    <mergeCell ref="S11:U12"/>
-    <mergeCell ref="V13:Y13"/>
-    <mergeCell ref="V14:Y14"/>
-    <mergeCell ref="V15:Y15"/>
-    <mergeCell ref="V16:Y16"/>
-    <mergeCell ref="AD56:AE56"/>
-    <mergeCell ref="AF56:AH56"/>
-    <mergeCell ref="S55:U55"/>
-    <mergeCell ref="V55:Y55"/>
-    <mergeCell ref="Z55:AA55"/>
-    <mergeCell ref="AB55:AC55"/>
-    <mergeCell ref="AD55:AE55"/>
-    <mergeCell ref="AF55:AH55"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="S53:U54"/>
-    <mergeCell ref="V53:Y54"/>
-    <mergeCell ref="Z53:AE53"/>
-    <mergeCell ref="AF53:AH54"/>
-    <mergeCell ref="Z54:AA54"/>
-    <mergeCell ref="AB54:AC54"/>
-    <mergeCell ref="AD54:AE54"/>
-    <mergeCell ref="V17:Y17"/>
-    <mergeCell ref="AF59:AH59"/>
-    <mergeCell ref="S58:U58"/>
-    <mergeCell ref="V58:Y58"/>
-    <mergeCell ref="Z58:AA58"/>
-    <mergeCell ref="AB58:AC58"/>
-    <mergeCell ref="AD58:AE58"/>
-    <mergeCell ref="AF58:AH58"/>
-    <mergeCell ref="S57:U57"/>
-    <mergeCell ref="V57:Y57"/>
-    <mergeCell ref="Z57:AA57"/>
-    <mergeCell ref="AB57:AC57"/>
-    <mergeCell ref="AD57:AE57"/>
-    <mergeCell ref="AF57:AH57"/>
-    <mergeCell ref="P52:R52"/>
-    <mergeCell ref="P53:R54"/>
-    <mergeCell ref="P55:R55"/>
-    <mergeCell ref="P56:R56"/>
-    <mergeCell ref="P57:R57"/>
-    <mergeCell ref="S59:U59"/>
-    <mergeCell ref="V59:Y59"/>
-    <mergeCell ref="Z59:AA59"/>
-    <mergeCell ref="AB59:AC59"/>
-    <mergeCell ref="S56:U56"/>
-    <mergeCell ref="V56:Y56"/>
-    <mergeCell ref="Z56:AA56"/>
-    <mergeCell ref="AB56:AC56"/>
-    <mergeCell ref="Q103:S103"/>
-    <mergeCell ref="T103:V103"/>
-    <mergeCell ref="W103:Z103"/>
-    <mergeCell ref="AA103:AB103"/>
-    <mergeCell ref="AC103:AD103"/>
-    <mergeCell ref="AE103:AF103"/>
-    <mergeCell ref="P58:R58"/>
-    <mergeCell ref="P59:R59"/>
-    <mergeCell ref="Q101:S102"/>
-    <mergeCell ref="T101:V102"/>
-    <mergeCell ref="W101:Z102"/>
-    <mergeCell ref="AA101:AF101"/>
-    <mergeCell ref="AD59:AE59"/>
-    <mergeCell ref="T104:V104"/>
-    <mergeCell ref="W104:Z104"/>
-    <mergeCell ref="AA104:AB104"/>
-    <mergeCell ref="AC104:AD104"/>
-    <mergeCell ref="AE104:AF104"/>
-    <mergeCell ref="AG104:AI104"/>
-    <mergeCell ref="AG101:AI102"/>
-    <mergeCell ref="AA102:AB102"/>
-    <mergeCell ref="AC102:AD102"/>
-    <mergeCell ref="AE102:AF102"/>
-    <mergeCell ref="AG107:AI107"/>
-    <mergeCell ref="N43:AL44"/>
-    <mergeCell ref="Q107:S107"/>
-    <mergeCell ref="T107:V107"/>
-    <mergeCell ref="W107:Z107"/>
-    <mergeCell ref="AA107:AB107"/>
-    <mergeCell ref="AC107:AD107"/>
-    <mergeCell ref="AE107:AF107"/>
-    <mergeCell ref="AG105:AI105"/>
-    <mergeCell ref="Q106:S106"/>
-    <mergeCell ref="T106:V106"/>
-    <mergeCell ref="W106:Z106"/>
-    <mergeCell ref="AA106:AB106"/>
-    <mergeCell ref="AC106:AD106"/>
-    <mergeCell ref="AE106:AF106"/>
-    <mergeCell ref="AG106:AI106"/>
-    <mergeCell ref="Q105:S105"/>
-    <mergeCell ref="T105:V105"/>
-    <mergeCell ref="W105:Z105"/>
-    <mergeCell ref="AA105:AB105"/>
-    <mergeCell ref="AC105:AD105"/>
-    <mergeCell ref="AE105:AF105"/>
-    <mergeCell ref="AG103:AI103"/>
-    <mergeCell ref="Q104:S104"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>